<commit_message>
womens 2023 test... corrected times to UTC
</commit_message>
<xml_diff>
--- a/tournaments/2023-womens-world-cup.xlsx
+++ b/tournaments/2023-womens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DA30AD-AD94-4F6F-8159-63E7CEE0446D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA82F4-6F73-466D-9C4E-286035A53B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1273" yWindow="1560" windowWidth="19200" windowHeight="10020" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="6400" yWindow="947" windowWidth="19200" windowHeight="10073" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>45127.708333333336</v>
+        <v>45127.291666666672</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1547,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>45127.833333333336</v>
+        <v>45127.416666666672</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1568,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>45128.625</v>
+        <v>45128.208333333336</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1589,7 +1589,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>45128.520833333336</v>
+        <v>45128.104166666672</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1610,7 +1610,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1">
-        <v>45128.729166666664</v>
+        <v>45128.3125</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1631,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>45129.708333333336</v>
+        <v>45129.291666666672</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1652,7 +1652,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="1">
-        <v>45129.8125</v>
+        <v>45129.395833333336</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1673,7 +1673,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <v>45129.916666666664</v>
+        <v>45129.5</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1694,7 +1694,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="1">
-        <v>45129.458333333336</v>
+        <v>45129.041666666672</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1715,7 +1715,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="1">
-        <v>45130.729166666664</v>
+        <v>45130.3125</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -1736,7 +1736,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="1">
-        <v>45130.833333333336</v>
+        <v>45130.416666666672</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1757,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="1">
-        <v>45130.625</v>
+        <v>45130.208333333336</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1778,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="1">
-        <v>45131.875</v>
+        <v>45131.458333333336</v>
       </c>
       <c r="E14">
         <v>9</v>
@@ -1799,7 +1799,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>45131.666666666664</v>
+        <v>45131.25</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1820,7 +1820,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="1">
-        <v>45131.770833333336</v>
+        <v>45131.354166666672</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1841,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="1">
-        <v>45132.5</v>
+        <v>45132.083333333336</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1862,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>45132.645833333336</v>
+        <v>45132.229166666672</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>45132.75</v>
+        <v>45132.333333333336</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1904,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>45133.916666666664</v>
+        <v>45133.5</v>
       </c>
       <c r="E20">
         <v>8</v>
@@ -1925,7 +1925,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="1">
-        <v>45133.729166666664</v>
+        <v>45133.3125</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1946,7 +1946,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="1">
-        <v>45133.625</v>
+        <v>45133.208333333336</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -1967,7 +1967,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>45134.833333333336</v>
+        <v>45134.416666666672</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -1988,7 +1988,7 @@
         <v>20</v>
       </c>
       <c r="D24" s="1">
-        <v>45134.458333333336</v>
+        <v>45134.041666666672</v>
       </c>
       <c r="E24">
         <v>5</v>
@@ -2009,7 +2009,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="1">
-        <v>45134.729166666664</v>
+        <v>45134.3125</v>
       </c>
       <c r="E25">
         <v>6</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="1">
-        <v>45135.770833333336</v>
+        <v>45135.354166666672</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2051,7 +2051,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="1">
-        <v>45135.875</v>
+        <v>45135.458333333336</v>
       </c>
       <c r="E27">
         <v>9</v>
@@ -2072,7 +2072,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="1">
-        <v>45135.416666666664</v>
+        <v>45135</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -2093,7 +2093,7 @@
         <v>22</v>
       </c>
       <c r="D29" s="1">
-        <v>45136.833333333336</v>
+        <v>45136.416666666672</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -2114,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="1">
-        <v>45136.9375</v>
+        <v>45136.520833333336</v>
       </c>
       <c r="E30">
         <v>8</v>
@@ -2135,7 +2135,7 @@
         <v>24</v>
       </c>
       <c r="D31" s="1">
-        <v>45136.729166666664</v>
+        <v>45136.3125</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -2156,7 +2156,7 @@
         <v>26</v>
       </c>
       <c r="D32" s="1">
-        <v>45137.8125</v>
+        <v>45137.395833333336</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -2177,7 +2177,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="1">
-        <v>45137.604166666664</v>
+        <v>45137.1875</v>
       </c>
       <c r="E33">
         <v>9</v>
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>45137.708333333336</v>
+        <v>45137.291666666672</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -2219,7 +2219,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>45137.708333333336</v>
+        <v>45137.291666666672</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -2240,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="1">
-        <v>45138.833333333336</v>
+        <v>45138.416666666672</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -2261,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="1">
-        <v>45138.833333333336</v>
+        <v>45138.416666666672</v>
       </c>
       <c r="E37">
         <v>7</v>
@@ -2282,7 +2282,7 @@
         <v>14</v>
       </c>
       <c r="D38" s="1">
-        <v>45138.708333333336</v>
+        <v>45138.291666666672</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -2303,7 +2303,7 @@
         <v>12</v>
       </c>
       <c r="D39" s="1">
-        <v>45138.708333333336</v>
+        <v>45138.291666666672</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -2324,7 +2324,7 @@
         <v>8</v>
       </c>
       <c r="D40" s="1">
-        <v>45139.875</v>
+        <v>45139.458333333336</v>
       </c>
       <c r="E40">
         <v>9</v>
@@ -2345,7 +2345,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="1">
-        <v>45139.875</v>
+        <v>45139.458333333336</v>
       </c>
       <c r="E41">
         <v>8</v>
@@ -2366,7 +2366,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="1">
-        <v>45139.708333333336</v>
+        <v>45139.291666666672</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2387,7 +2387,7 @@
         <v>20</v>
       </c>
       <c r="D43" s="1">
-        <v>45139.708333333336</v>
+        <v>45139.291666666672</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -2408,7 +2408,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="1">
-        <v>45140.833333333336</v>
+        <v>45140.416666666672</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -2429,7 +2429,7 @@
         <v>22</v>
       </c>
       <c r="D45" s="1">
-        <v>45140.833333333336</v>
+        <v>45140.416666666672</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -2450,7 +2450,7 @@
         <v>30</v>
       </c>
       <c r="D46" s="1">
-        <v>45140.708333333336</v>
+        <v>45140.291666666672</v>
       </c>
       <c r="E46">
         <v>6</v>
@@ -2471,7 +2471,7 @@
         <v>24</v>
       </c>
       <c r="D47" s="1">
-        <v>45140.708333333336</v>
+        <v>45140.291666666672</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -2492,7 +2492,7 @@
         <v>28</v>
       </c>
       <c r="D48" s="1">
-        <v>45141.833333333336</v>
+        <v>45141.416666666672</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -2513,7 +2513,7 @@
         <v>26</v>
       </c>
       <c r="D49" s="1">
-        <v>45141.833333333336</v>
+        <v>45141.416666666672</v>
       </c>
       <c r="E49">
         <v>8</v>
@@ -2534,7 +2534,7 @@
         <v>39</v>
       </c>
       <c r="D50" s="1">
-        <v>45143.625</v>
+        <v>45143.208333333336</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2555,7 +2555,7 @@
         <v>37</v>
       </c>
       <c r="D51" s="1">
-        <v>45143.75</v>
+        <v>45143.333333333336</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -2576,7 +2576,7 @@
         <v>47</v>
       </c>
       <c r="D52" s="1">
-        <v>45144.5</v>
+        <v>45144.083333333336</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -2597,7 +2597,7 @@
         <v>45</v>
       </c>
       <c r="D53" s="1">
-        <v>45144.791666666664</v>
+        <v>45144.375</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -2618,7 +2618,7 @@
         <v>35</v>
       </c>
       <c r="D54" s="1">
-        <v>45145.854166666664</v>
+        <v>45145.4375</v>
       </c>
       <c r="E54">
         <v>10</v>
@@ -2639,7 +2639,7 @@
         <v>33</v>
       </c>
       <c r="D55" s="1">
-        <v>45145.729166666664</v>
+        <v>45145.3125</v>
       </c>
       <c r="E55">
         <v>7</v>
@@ -2660,7 +2660,7 @@
         <v>43</v>
       </c>
       <c r="D56" s="1">
-        <v>45146.875</v>
+        <v>45146.458333333336</v>
       </c>
       <c r="E56">
         <v>9</v>
@@ -2681,7 +2681,7 @@
         <v>41</v>
       </c>
       <c r="D57" s="1">
-        <v>45146.75</v>
+        <v>45146.333333333336</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -2702,7 +2702,7 @@
         <v>52</v>
       </c>
       <c r="D58" s="1">
-        <v>45149.458333333336</v>
+        <v>45149.041666666672</v>
       </c>
       <c r="E58">
         <v>5</v>
@@ -2723,7 +2723,7 @@
         <v>53</v>
       </c>
       <c r="D59" s="1">
-        <v>45149.729166666664</v>
+        <v>45149.3125</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2744,7 +2744,7 @@
         <v>54</v>
       </c>
       <c r="D60" s="1">
-        <v>45150.708333333336</v>
+        <v>45150.291666666672</v>
       </c>
       <c r="E60">
         <v>7</v>
@@ -2765,7 +2765,7 @@
         <v>55</v>
       </c>
       <c r="D61" s="1">
-        <v>45150.854166666664</v>
+        <v>45150.4375</v>
       </c>
       <c r="E61">
         <v>10</v>
@@ -2786,7 +2786,7 @@
         <v>57</v>
       </c>
       <c r="D62" s="1">
-        <v>45153.75</v>
+        <v>45153.333333333336</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2807,7 +2807,7 @@
         <v>59</v>
       </c>
       <c r="D63" s="1">
-        <v>45154.833333333336</v>
+        <v>45154.416666666672</v>
       </c>
       <c r="E63">
         <v>10</v>
@@ -2828,7 +2828,7 @@
         <v>85</v>
       </c>
       <c r="D64" s="1">
-        <v>45157.75</v>
+        <v>45157.333333333336</v>
       </c>
       <c r="E64">
         <v>7</v>
@@ -2849,7 +2849,7 @@
         <v>61</v>
       </c>
       <c r="D65" s="1">
-        <v>45158.833333333336</v>
+        <v>45158.416666666672</v>
       </c>
       <c r="E65">
         <v>10</v>
@@ -2860,6 +2860,7 @@
       <c r="K65" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>